<commit_message>
Translation works on toReport values and fromReport values
More AOE fields
</commit_message>
<xml_diff>
--- a/prime-router/docs/schema_mappings/12_29 PA DOH __ STRAX PRIME HL7 Mapping.xlsx
+++ b/prime-router/docs/schema_mappings/12_29 PA DOH __ STRAX PRIME HL7 Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rickhawes/Projects/prime-data-hub/prime-router/docs/schema_mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FF1F69-9CAD-A14A-940F-B61DF11CA390}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A22684-F222-7D45-8160-9A22995F439F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25620" yWindow="500" windowWidth="25600" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1298,9 +1298,9 @@
   </sheetPr>
   <dimension ref="A1:AC988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -1411,7 +1411,7 @@
       <c r="B3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="25" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="27" t="s">
@@ -2203,7 +2203,7 @@
       <c r="B22" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="25" t="s">
         <v>77</v>
       </c>
       <c r="D22" s="27"/>
@@ -2448,7 +2448,7 @@
       <c r="B28" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="25" t="s">
         <v>39</v>
       </c>
       <c r="D28" s="24" t="s">
@@ -3510,7 +3510,7 @@
       <c r="A54" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="25" t="s">
         <v>204</v>
       </c>
       <c r="C54" s="7"/>
@@ -3755,7 +3755,7 @@
       <c r="B60" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="25" t="s">
         <v>223</v>
       </c>
       <c r="D60" s="24" t="s">

</xml_diff>